<commit_message>
group admins by course
</commit_message>
<xml_diff>
--- a/mssa_dot_test.xlsx
+++ b/mssa_dot_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/narwhal/Local/echidna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C674B39-8172-0647-8CFC-C1ED2F6A17B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C46B73B-21F9-A741-844D-768B7A905FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2800" yWindow="4460" windowWidth="29400" windowHeight="18360" xr2:uid="{C5C2C06C-AB47-4043-8CF2-15AF3C90E20F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
   <si>
     <t>PAT_ENC_CSN_ID</t>
   </si>
@@ -433,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4DB316-8676-F74E-B994-F79FFE6AED59}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,11 +510,11 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3">
-        <v>44592.892361111109</v>
+      <c r="C5" s="1">
+        <v>44586.724803240744</v>
       </c>
       <c r="D5" s="1">
-        <v>44594.205555555556</v>
+        <v>44586.766469907408</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -522,13 +522,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
-        <v>44586.122361111113</v>
+        <v>44587.724803240744</v>
       </c>
       <c r="D6" s="1">
-        <v>44586.629120370373</v>
+        <v>44587.808136574073</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -536,13 +536,13 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1">
-        <v>44586.899375000001</v>
+        <v>3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>44592.892361111109</v>
       </c>
       <c r="D7" s="1">
-        <v>44588.438194444447</v>
+        <v>44594.205555555556</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -550,13 +550,13 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1">
-        <v>44588.691377314812</v>
+        <v>44595.205555555556</v>
       </c>
       <c r="D8" s="1">
-        <v>44589.422314814816</v>
+        <v>44595.24722222222</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -564,26 +564,96 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1">
-        <v>44589.696817129632</v>
+        <v>44596.205555555556</v>
       </c>
       <c r="D9" s="1">
-        <v>44592.608263888891</v>
+        <v>44596.288888888892</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44598.205555555556</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44598.288888888892</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44586.122361111113</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44586.629120370373</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44586.899375000001</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44588.438194444447</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44588.691377314812</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44589.422314814816</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1">
+        <v>44589.696817129632</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44592.608263888891</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B15" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C15" s="2">
         <v>44589</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D15" s="2">
         <v>44592</v>
       </c>
     </row>

</xml_diff>